<commit_message>
feat：udpate new tower and world5
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Item_道具表.xlsx
+++ b/nevergiveup/Excel/Item_道具表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -514,7 +514,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3142,13 +3142,23 @@
       <c r="AH20" s="12"/>
       <c r="AK20" s="12"/>
     </row>
-    <row r="21" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
+    <row r="21" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="n">
+        <v>1012</v>
+      </c>
+      <c r="B21" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="15" t="n">
+        <v>1012</v>
+      </c>
+      <c r="D21" s="15" t="n">
+        <v>2</v>
+      </c>
       <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="F21" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
       <c r="R21" s="12"/>

</xml_diff>

<commit_message>
feat：update 2 new tower
上传两个新防御塔
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Item_道具表.xlsx
+++ b/nevergiveup/Excel/Item_道具表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -514,7 +514,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3168,13 +3168,23 @@
       <c r="AH21" s="12"/>
       <c r="AK21" s="14"/>
     </row>
-    <row r="22" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+    <row r="22" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="n">
+        <v>1013</v>
+      </c>
+      <c r="B22" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="15" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D22" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" s="15"/>
+      <c r="F22" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="R22" s="14"/>
       <c r="AC22" s="13"/>
       <c r="AD22" s="14"/>

</xml_diff>

<commit_message>
feat：update 3 new tower
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Item_道具表.xlsx
+++ b/nevergiveup/Excel/Item_道具表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -514,7 +514,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3192,25 +3192,45 @@
       <c r="AH22" s="12"/>
       <c r="AK22" s="12"/>
     </row>
-    <row r="23" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
+    <row r="23" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="n">
+        <v>1014</v>
+      </c>
+      <c r="B23" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="15" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D23" s="15" t="n">
+        <v>2</v>
+      </c>
       <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
+      <c r="F23" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
       <c r="AC23" s="13"/>
       <c r="AE23" s="13"/>
     </row>
-    <row r="24" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+    <row r="24" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="n">
+        <v>1015</v>
+      </c>
+      <c r="B24" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="15" t="n">
+        <v>1015</v>
+      </c>
+      <c r="D24" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" s="15"/>
+      <c r="F24" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="R24" s="12"/>
       <c r="AC24" s="13"/>
       <c r="AD24" s="12"/>

</xml_diff>

<commit_message>
feat：update dark dragon 2
提交暗龙娘2
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Item_道具表.xlsx
+++ b/nevergiveup/Excel/Item_道具表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -514,7 +514,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3280,13 +3280,23 @@
       <c r="AC26" s="9"/>
       <c r="AE26" s="9"/>
     </row>
-    <row r="27" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+    <row r="27" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>1018</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>1018</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="F27" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="S27" s="9"/>
       <c r="AC27" s="9"/>
       <c r="AE27" s="9"/>

</xml_diff>

<commit_message>
feat：update tower and TaskMain fix
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Item_道具表.xlsx
+++ b/nevergiveup/Excel/Item_道具表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -514,7 +514,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+      <selection pane="bottomLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3301,24 +3301,44 @@
       <c r="AC27" s="9"/>
       <c r="AE27" s="9"/>
     </row>
-    <row r="28" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+    <row r="28" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>1019</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>1019</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="F28" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="S28" s="9"/>
       <c r="AC28" s="9"/>
       <c r="AE28" s="9"/>
     </row>
-    <row r="29" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+    <row r="29" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>1020</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>1020</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="F29" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="S29" s="9"/>
       <c r="AC29" s="9"/>
       <c r="AE29" s="9"/>

</xml_diff>

<commit_message>
feat：update new water tower
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Item_道具表.xlsx
+++ b/nevergiveup/Excel/Item_道具表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -514,7 +514,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
+      <selection pane="bottomLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3490,24 +3490,44 @@
       <c r="AC36" s="9"/>
       <c r="AE36" s="9"/>
     </row>
-    <row r="37" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
+    <row r="37" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="n">
+        <v>1028</v>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>1028</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="F37" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="S37" s="9"/>
       <c r="AC37" s="9"/>
       <c r="AE37" s="9"/>
     </row>
-    <row r="38" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+    <row r="38" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="n">
+        <v>1029</v>
+      </c>
+      <c r="B38" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>1029</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+      <c r="F38" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="S38" s="9"/>
       <c r="AC38" s="9"/>
       <c r="AE38" s="9"/>

</xml_diff>

<commit_message>
feat：update water tower 1030
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Item_道具表.xlsx
+++ b/nevergiveup/Excel/Item_道具表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -514,7 +514,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
+      <selection pane="bottomLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3532,13 +3532,23 @@
       <c r="AC38" s="9"/>
       <c r="AE38" s="9"/>
     </row>
-    <row r="39" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
+    <row r="39" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="n">
+        <v>1030</v>
+      </c>
+      <c r="B39" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>1030</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+      <c r="F39" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="S39" s="9"/>
       <c r="AC39" s="9"/>
       <c r="AE39" s="9"/>

</xml_diff>

<commit_message>
feat：update firedragon prefab and tower excel
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Item_道具表.xlsx
+++ b/nevergiveup/Excel/Item_道具表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -512,9 +512,9 @@
   <dimension ref="A1:AMJ377"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
+      <selection pane="bottomLeft" activeCell="H42" activeCellId="0" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3553,13 +3553,23 @@
       <c r="AC39" s="9"/>
       <c r="AE39" s="9"/>
     </row>
-    <row r="40" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
+    <row r="40" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="n">
+        <v>1031</v>
+      </c>
+      <c r="B40" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>1031</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="F40" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="S40" s="9"/>
       <c r="AC40" s="9"/>
       <c r="AE40" s="9"/>

</xml_diff>